<commit_message>
feat(it4-planning): uploading planning info
</commit_message>
<xml_diff>
--- a/iteración-4/resources/Planning.xlsx
+++ b/iteración-4/resources/Planning.xlsx
@@ -462,14 +462,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -777,7 +777,7 @@
   <dimension ref="A2:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,42 +787,42 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="21" t="s">
+      <c r="B3" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="21" t="s">
+      <c r="E3" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="J3" s="19" t="s">
+      <c r="H3" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="17" t="s">
         <v>9</v>
       </c>
     </row>
@@ -830,7 +830,9 @@
       <c r="A4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2">
+        <v>2</v>
+      </c>
       <c r="C4" s="2">
         <v>3</v>
       </c>
@@ -843,17 +845,23 @@
       <c r="F4" s="2">
         <v>2</v>
       </c>
-      <c r="G4" s="2"/>
+      <c r="G4" s="2">
+        <v>3</v>
+      </c>
       <c r="H4" s="2">
         <v>3</v>
       </c>
-      <c r="J4" s="2"/>
+      <c r="J4" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="1">
+        <v>8</v>
+      </c>
       <c r="C5" s="1">
         <v>13</v>
       </c>
@@ -866,17 +874,23 @@
       <c r="F5" s="1">
         <v>8</v>
       </c>
-      <c r="G5" s="1"/>
+      <c r="G5" s="1">
+        <v>8</v>
+      </c>
       <c r="H5" s="1">
         <v>13</v>
       </c>
-      <c r="J5" s="1"/>
+      <c r="J5" s="1">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="1">
+        <v>5</v>
+      </c>
       <c r="C6" s="1">
         <v>8</v>
       </c>
@@ -889,17 +903,23 @@
       <c r="F6" s="1">
         <v>5</v>
       </c>
-      <c r="G6" s="1"/>
+      <c r="G6" s="1">
+        <v>8</v>
+      </c>
       <c r="H6" s="1">
         <v>8</v>
       </c>
-      <c r="J6" s="1"/>
+      <c r="J6" s="1">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="1">
+        <v>8</v>
+      </c>
       <c r="C7" s="1">
         <v>8</v>
       </c>
@@ -912,17 +932,23 @@
       <c r="F7" s="1">
         <v>8</v>
       </c>
-      <c r="G7" s="1"/>
+      <c r="G7" s="1">
+        <v>8</v>
+      </c>
       <c r="H7" s="1">
         <v>8</v>
       </c>
-      <c r="J7" s="1"/>
+      <c r="J7" s="1">
+        <v>8</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="1">
+        <v>3</v>
+      </c>
       <c r="C8" s="1">
         <v>2</v>
       </c>
@@ -935,11 +961,15 @@
       <c r="F8" s="1">
         <v>5</v>
       </c>
-      <c r="G8" s="1"/>
+      <c r="G8" s="1">
+        <v>3</v>
+      </c>
       <c r="H8" s="1">
         <v>3</v>
       </c>
-      <c r="J8" s="1"/>
+      <c r="J8" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
@@ -986,15 +1016,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -1717,15 +1747,15 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>

</xml_diff>